<commit_message>
Début affectation de tâches... A voir demain
</commit_message>
<xml_diff>
--- a/Documentation/Planification - Schéma GANTT initial.xlsx
+++ b/Documentation/Planification - Schéma GANTT initial.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="156" windowWidth="20052" windowHeight="12012"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="20055" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="102">
   <si>
     <t>Tâche</t>
   </si>
@@ -319,6 +322,9 @@
   </si>
   <si>
     <t>Vacances de Noël</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -853,8 +859,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1153,26 +1187,26 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="0.44140625" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" style="6" customWidth="1"/>
-    <col min="8" max="19" width="5.109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="5.109375" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" style="6" customWidth="1"/>
+    <col min="8" max="19" width="5.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:20" ht="25.9" x14ac:dyDescent="0.5">
       <c r="A1" s="58" t="s">
         <v>21</v>
       </c>
@@ -1182,7 +1216,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:20" s="16" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="16" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="62" t="s">
         <v>78</v>
       </c>
@@ -1207,7 +1241,7 @@
       <c r="S2" s="55"/>
       <c r="T2" s="56"/>
     </row>
-    <row r="3" spans="1:20" s="15" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
       <c r="B3" s="18" t="s">
         <v>0</v>
@@ -1265,7 +1299,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>22</v>
       </c>
@@ -1291,7 +1325,7 @@
       <c r="S4" s="35"/>
       <c r="T4" s="36"/>
     </row>
-    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="10" t="s">
         <v>3</v>
@@ -1321,7 +1355,7 @@
       <c r="S5" s="31"/>
       <c r="T5" s="31"/>
     </row>
-    <row r="6" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="10" t="s">
         <v>4</v>
@@ -1329,7 +1363,9 @@
       <c r="C6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="E6" s="7">
         <v>1</v>
       </c>
@@ -1349,7 +1385,7 @@
       <c r="S6" s="31"/>
       <c r="T6" s="31"/>
     </row>
-    <row r="7" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="10" t="s">
         <v>5</v>
@@ -1377,7 +1413,7 @@
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
     </row>
-    <row r="8" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="10" t="s">
         <v>6</v>
@@ -1407,7 +1443,7 @@
       <c r="S8" s="31"/>
       <c r="T8" s="31"/>
     </row>
-    <row r="9" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>7</v>
@@ -1437,7 +1473,7 @@
       <c r="S9" s="31"/>
       <c r="T9" s="31"/>
     </row>
-    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
         <v>26</v>
       </c>
@@ -1463,7 +1499,7 @@
       <c r="S10" s="31"/>
       <c r="T10" s="31"/>
     </row>
-    <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>8</v>
@@ -1471,7 +1507,9 @@
       <c r="C11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="E11" s="11">
         <v>1</v>
       </c>
@@ -1491,7 +1529,7 @@
       <c r="S11" s="31"/>
       <c r="T11" s="31"/>
     </row>
-    <row r="12" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>9</v>
@@ -1519,7 +1557,7 @@
       <c r="S12" s="31"/>
       <c r="T12" s="31"/>
     </row>
-    <row r="13" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>10</v>
@@ -1527,7 +1565,9 @@
       <c r="C13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="E13" s="33">
         <v>2</v>
       </c>
@@ -1547,7 +1587,7 @@
       <c r="S13" s="31"/>
       <c r="T13" s="31"/>
     </row>
-    <row r="14" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="10" t="s">
         <v>63</v>
@@ -1555,7 +1595,9 @@
       <c r="C14" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="E14" s="12">
         <v>1</v>
       </c>
@@ -1575,7 +1617,7 @@
       <c r="S14" s="31"/>
       <c r="T14" s="31"/>
     </row>
-    <row r="15" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="10" t="s">
         <v>64</v>
@@ -1583,7 +1625,9 @@
       <c r="C15" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="E15" s="12">
         <v>1</v>
       </c>
@@ -1603,7 +1647,7 @@
       <c r="S15" s="31"/>
       <c r="T15" s="31"/>
     </row>
-    <row r="16" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="10" t="s">
         <v>11</v>
@@ -1631,7 +1675,7 @@
       <c r="S16" s="40"/>
       <c r="T16" s="40"/>
     </row>
-    <row r="17" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="10" t="s">
         <v>66</v>
@@ -1659,7 +1703,7 @@
       <c r="S17" s="40"/>
       <c r="T17" s="40"/>
     </row>
-    <row r="18" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="10" t="s">
         <v>67</v>
@@ -1687,7 +1731,7 @@
       <c r="S18" s="40"/>
       <c r="T18" s="40"/>
     </row>
-    <row r="19" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="10" t="s">
         <v>82</v>
@@ -1715,7 +1759,7 @@
       <c r="S19" s="31"/>
       <c r="T19" s="31"/>
     </row>
-    <row r="20" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="27" t="s">
         <v>83</v>
@@ -1743,7 +1787,7 @@
       <c r="S20" s="31"/>
       <c r="T20" s="31"/>
     </row>
-    <row r="21" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="27" t="s">
         <v>84</v>
@@ -1771,7 +1815,7 @@
       <c r="S21" s="31"/>
       <c r="T21" s="31"/>
     </row>
-    <row r="22" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="53" t="s">
         <v>27</v>
       </c>
@@ -1797,7 +1841,7 @@
       <c r="S22" s="31"/>
       <c r="T22" s="31"/>
     </row>
-    <row r="23" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>85</v>
@@ -1825,7 +1869,7 @@
       <c r="S23" s="40"/>
       <c r="T23" s="40"/>
     </row>
-    <row r="24" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="10" t="s">
         <v>86</v>
@@ -1853,7 +1897,7 @@
       <c r="S24" s="40"/>
       <c r="T24" s="40"/>
     </row>
-    <row r="25" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="10" t="s">
         <v>87</v>
@@ -1881,7 +1925,7 @@
       <c r="S25" s="40"/>
       <c r="T25" s="40"/>
     </row>
-    <row r="26" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="10" t="s">
         <v>88</v>
@@ -1909,7 +1953,7 @@
       <c r="S26" s="40"/>
       <c r="T26" s="40"/>
     </row>
-    <row r="27" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F27" s="22"/>
       <c r="G27" s="57" t="s">
         <v>54</v>
@@ -1928,7 +1972,7 @@
       <c r="S27" s="57"/>
       <c r="T27" s="57"/>
     </row>
-    <row r="28" spans="1:20" s="23" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" s="23" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="18" t="s">
         <v>0</v>
@@ -1984,7 +2028,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="10" t="s">
         <v>89</v>
@@ -2012,7 +2056,7 @@
       <c r="S29" s="40"/>
       <c r="T29" s="40"/>
     </row>
-    <row r="30" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="10" t="s">
         <v>90</v>
@@ -2040,7 +2084,7 @@
       <c r="S30" s="40"/>
       <c r="T30" s="40"/>
     </row>
-    <row r="31" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="10" t="s">
         <v>91</v>
@@ -2068,7 +2112,7 @@
       <c r="S31" s="40"/>
       <c r="T31" s="40"/>
     </row>
-    <row r="32" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="10" t="s">
         <v>12</v>
@@ -2096,7 +2140,7 @@
       <c r="S32" s="40"/>
       <c r="T32" s="40"/>
     </row>
-    <row r="33" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
       <c r="B33" s="27" t="s">
         <v>92</v>
@@ -2124,7 +2168,7 @@
       <c r="S33" s="40"/>
       <c r="T33" s="40"/>
     </row>
-    <row r="34" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="27" t="s">
         <v>93</v>
@@ -2152,7 +2196,7 @@
       <c r="S34" s="40"/>
       <c r="T34" s="40"/>
     </row>
-    <row r="35" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="26"/>
       <c r="B35" s="27" t="s">
         <v>94</v>
@@ -2180,7 +2224,7 @@
       <c r="S35" s="40"/>
       <c r="T35" s="40"/>
     </row>
-    <row r="36" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="27" t="s">
         <v>95</v>
@@ -2208,7 +2252,7 @@
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
     </row>
-    <row r="37" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
       <c r="B37" s="27" t="s">
         <v>96</v>
@@ -2216,7 +2260,9 @@
       <c r="C37" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="E37" s="28">
         <v>1</v>
       </c>
@@ -2236,7 +2282,7 @@
       <c r="S37" s="40"/>
       <c r="T37" s="40"/>
     </row>
-    <row r="38" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="27" t="s">
         <v>97</v>
@@ -2264,7 +2310,7 @@
       <c r="S38" s="40"/>
       <c r="T38" s="40"/>
     </row>
-    <row r="39" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="53" t="s">
         <v>30</v>
       </c>
@@ -2288,7 +2334,7 @@
       <c r="S39" s="31"/>
       <c r="T39" s="31"/>
     </row>
-    <row r="40" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="10" t="s">
         <v>13</v>
@@ -2316,7 +2362,7 @@
       <c r="S40" s="40"/>
       <c r="T40" s="40"/>
     </row>
-    <row r="41" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="10" t="s">
         <v>14</v>
@@ -2344,7 +2390,7 @@
       <c r="S41" s="40"/>
       <c r="T41" s="40"/>
     </row>
-    <row r="42" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="10" t="s">
         <v>15</v>
@@ -2372,7 +2418,7 @@
       <c r="S42" s="40"/>
       <c r="T42" s="40"/>
     </row>
-    <row r="43" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="53" t="s">
         <v>34</v>
       </c>
@@ -2396,7 +2442,7 @@
       <c r="S43" s="31"/>
       <c r="T43" s="31"/>
     </row>
-    <row r="44" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="10" t="s">
         <v>16</v>
@@ -2424,7 +2470,7 @@
       <c r="S44" s="48"/>
       <c r="T44" s="40"/>
     </row>
-    <row r="45" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="10" t="s">
         <v>17</v>
@@ -2452,7 +2498,7 @@
       <c r="S45" s="48"/>
       <c r="T45" s="40"/>
     </row>
-    <row r="46" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="10" t="s">
         <v>18</v>
@@ -2480,7 +2526,7 @@
       <c r="S46" s="48"/>
       <c r="T46" s="40"/>
     </row>
-    <row r="47" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="10" t="s">
         <v>19</v>
@@ -2508,7 +2554,7 @@
       <c r="S47" s="48"/>
       <c r="T47" s="40"/>
     </row>
-    <row r="48" spans="1:20" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="10" t="s">
         <v>20</v>
@@ -2536,14 +2582,14 @@
       <c r="S48" s="40"/>
       <c r="T48" s="48"/>
     </row>
-    <row r="49" spans="3:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
     </row>
-    <row r="50" spans="3:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C50" s="25"/>
       <c r="D50" s="25"/>
     </row>
@@ -2574,7 +2620,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2586,7 +2632,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>